<commit_message>
Generated CAM, BOM and CPL files
</commit_message>
<xml_diff>
--- a/cam/RP2040-ProMini-20230716-JLCPCB-BOM-WSON.xlsx
+++ b/cam/RP2040-ProMini-20230716-JLCPCB-BOM-WSON.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AG\Documents\KiCad\7.0\projects\RP2040-ProMini\cam\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DD9E35D-A2CB-4007-9C5A-B9CE1EABE6CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4AD13CB-6151-401C-8AE8-0500CC4E3C08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22536" yWindow="1620" windowWidth="19656" windowHeight="21684" xr2:uid="{1A36A938-FF2D-482B-8DC2-6C784DBF3E37}"/>
+    <workbookView xWindow="26292" yWindow="3276" windowWidth="19656" windowHeight="21684" xr2:uid="{1A36A938-FF2D-482B-8DC2-6C784DBF3E37}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -118,9 +118,6 @@
     <t>0402</t>
   </si>
   <si>
-    <t>SOIC-8-208mil</t>
-  </si>
-  <si>
     <t>C2040</t>
   </si>
   <si>
@@ -236,6 +233,9 @@
   </si>
   <si>
     <t>1.5uH</t>
+  </si>
+  <si>
+    <t>WSON-8-EP(6x8)</t>
   </si>
 </sst>
 </file>
@@ -602,7 +602,7 @@
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -643,7 +643,7 @@
         <v>20</v>
       </c>
       <c r="D2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E2" t="s">
         <v>3</v>
@@ -660,7 +660,7 @@
         <v>21</v>
       </c>
       <c r="D3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E3" t="s">
         <v>5</v>
@@ -671,13 +671,13 @@
         <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E4" t="s">
         <v>6</v>
@@ -688,16 +688,16 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E5" t="s">
         <v>51</v>
-      </c>
-      <c r="E5" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -705,13 +705,13 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E6" t="s">
         <v>9</v>
@@ -722,16 +722,16 @@
         <v>2</v>
       </c>
       <c r="B7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -739,16 +739,16 @@
         <v>1</v>
       </c>
       <c r="B8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D8" t="s">
+        <v>36</v>
+      </c>
+      <c r="E8" t="s">
         <v>35</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D8" t="s">
-        <v>37</v>
-      </c>
-      <c r="E8" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -756,16 +756,16 @@
         <v>1</v>
       </c>
       <c r="B9" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="D9" t="s">
         <v>39</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>40</v>
-      </c>
-      <c r="E9" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
@@ -776,10 +776,10 @@
         <v>10</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E10" t="s">
         <v>11</v>
@@ -793,10 +793,10 @@
         <v>12</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E11" t="s">
         <v>13</v>
@@ -810,10 +810,10 @@
         <v>14</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E12" t="s">
         <v>15</v>
@@ -824,16 +824,16 @@
         <v>1</v>
       </c>
       <c r="B13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D13" t="s">
+        <v>42</v>
+      </c>
+      <c r="E13" t="s">
         <v>43</v>
-      </c>
-      <c r="E13" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
@@ -841,16 +841,16 @@
         <v>2</v>
       </c>
       <c r="B14" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D14" t="s">
+        <v>53</v>
+      </c>
+      <c r="E14" t="s">
         <v>54</v>
-      </c>
-      <c r="E14" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
@@ -861,13 +861,13 @@
         <v>16</v>
       </c>
       <c r="C15" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D15" t="s">
         <v>56</v>
       </c>
-      <c r="D15" t="s">
+      <c r="E15" t="s">
         <v>57</v>
-      </c>
-      <c r="E15" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
@@ -881,7 +881,7 @@
         <v>21</v>
       </c>
       <c r="D16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E16" t="s">
         <v>8</v>
@@ -892,16 +892,16 @@
         <v>1</v>
       </c>
       <c r="B17" t="s">
+        <v>58</v>
+      </c>
+      <c r="C17" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="D17" t="s">
         <v>60</v>
       </c>
-      <c r="D17" t="s">
+      <c r="E17" t="s">
         <v>61</v>
-      </c>
-      <c r="E17" t="s">
-        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>